<commit_message>
function one implementation and tests update
</commit_message>
<xml_diff>
--- a/documents/GE3_TestCases_2023_v1.0.xlsx
+++ b/documents/GE3_TestCases_2023_v1.0.xlsx
@@ -1,15 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\PycharmProjects\G01.2023.T04.EG3\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB561E07-E33E-4198-A129-6C09B7499E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-30" yWindow="0" windowWidth="9270" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="GE3 2023 F1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="GE3 2023 F2" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="GE3 2023 F3" sheetId="3" r:id="rId6"/>
+    <sheet name="GE3 2023 F1" sheetId="1" r:id="rId1"/>
+    <sheet name="GE3 2023 F2" sheetId="2" r:id="rId2"/>
+    <sheet name="GE3 2023 F3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgtDnqHNna3yI/VLx7bEZKKcCsFxA=="/>
     </ext>
@@ -349,48 +369,50 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="8">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
     </font>
@@ -400,7 +422,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -416,144 +438,173 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9E2F3"/>
           <bgColor rgb="FFD9E2F3"/>
         </patternFill>
       </fill>
-      <border/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="3">
-    <tableStyle count="3" pivot="0" name="GE3 2023 F1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    <tableStyle name="GE3 2023 F1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="GE3 2023 F2-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    <tableStyle name="GE3 2023 F2-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="GE3 2023 F3-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    <tableStyle name="GE3 2023 F3-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:AD44" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AD44" headerRowCount="0">
   <tableColumns count="30">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
-    <tableColumn name="Column3" id="3"/>
-    <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
-    <tableColumn name="Column6" id="6"/>
-    <tableColumn name="Column7" id="7"/>
-    <tableColumn name="Column8" id="8"/>
-    <tableColumn name="Column9" id="9"/>
-    <tableColumn name="Column10" id="10"/>
-    <tableColumn name="Column11" id="11"/>
-    <tableColumn name="Column12" id="12"/>
-    <tableColumn name="Column13" id="13"/>
-    <tableColumn name="Column14" id="14"/>
-    <tableColumn name="Column15" id="15"/>
-    <tableColumn name="Column16" id="16"/>
-    <tableColumn name="Column17" id="17"/>
-    <tableColumn name="Column18" id="18"/>
-    <tableColumn name="Column19" id="19"/>
-    <tableColumn name="Column20" id="20"/>
-    <tableColumn name="Column21" id="21"/>
-    <tableColumn name="Column22" id="22"/>
-    <tableColumn name="Column23" id="23"/>
-    <tableColumn name="Column24" id="24"/>
-    <tableColumn name="Column25" id="25"/>
-    <tableColumn name="Column26" id="26"/>
-    <tableColumn name="Column27" id="27"/>
-    <tableColumn name="Column28" id="28"/>
-    <tableColumn name="Column29" id="29"/>
-    <tableColumn name="Column30" id="30"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column21"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column23"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Column24"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Column25"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Column26"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Column27"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Column28"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Column29"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Column30"/>
   </tableColumns>
-  <tableStyleInfo name="GE3 2023 F1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="GE3 2023 F1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
@@ -563,40 +614,40 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J43" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:J43">
   <tableColumns count="10">
-    <tableColumn name="#" id="1"/>
-    <tableColumn name="NODE" id="2"/>
-    <tableColumn name="TERMINAL  (T) / NO TERMINAL (NT)" id="3"/>
-    <tableColumn name="TYPE (DUPLICATION / DELETION / MODIFICATION / VALID)" id="4"/>
-    <tableColumn name="ID TEST" id="5"/>
-    <tableColumn name="DESCRIPTION" id="6"/>
-    <tableColumn name="FILE PATH" id="7"/>
-    <tableColumn name="FILE CONTENT" id="8"/>
-    <tableColumn name="EXPECTED RESULT" id="9"/>
-    <tableColumn name="OBSERVATIONS" id="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="#"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NODE"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TERMINAL  (T) / NO TERMINAL (NT)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="TYPE (DUPLICATION / DELETION / MODIFICATION / VALID)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="ID TEST"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="DESCRIPTION"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="FILE PATH"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="FILE CONTENT"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="EXPECTED RESULT"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="OBSERVATIONS"/>
   </tableColumns>
-  <tableStyleInfo name="GE3 2023 F2-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="GE3 2023 F2-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G43" displayName="Table_3" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="A1:G43">
   <tableColumns count="7">
-    <tableColumn name="#" id="1"/>
-    <tableColumn name="PATH" id="2"/>
-    <tableColumn name="ID TEST" id="3"/>
-    <tableColumn name="DESCRIPTION" id="4"/>
-    <tableColumn name="KEY" id="5"/>
-    <tableColumn name="EXPECTED RESULT" id="6"/>
-    <tableColumn name="OBSERVATIONS" id="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="#"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="PATH"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ID TEST"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="DESCRIPTION"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="KEY"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="EXPECTED RESULT"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="OBSERVATIONS"/>
   </tableColumns>
-  <tableStyleInfo name="GE3 2023 F3-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="GE3 2023 F3-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -786,35 +837,37 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="10.1" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="10.07421875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="10.6"/>
-    <col customWidth="1" min="3" max="3" width="8.5"/>
-    <col customWidth="1" min="4" max="4" width="14.3"/>
-    <col customWidth="1" min="5" max="5" width="11.3"/>
-    <col customWidth="1" min="6" max="6" width="14.8"/>
-    <col customWidth="1" min="7" max="7" width="22.2"/>
-    <col customWidth="1" min="8" max="8" width="18.1"/>
-    <col customWidth="1" min="9" max="9" width="14.0"/>
-    <col customWidth="1" min="10" max="10" width="31.3"/>
-    <col customWidth="1" min="11" max="11" width="14.2"/>
-    <col customWidth="1" min="12" max="12" width="13.3"/>
-    <col customWidth="1" min="13" max="13" width="70.9"/>
-    <col customWidth="1" min="14" max="30" width="10.6"/>
+    <col min="1" max="2" width="10.61328125" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" customWidth="1"/>
+    <col min="5" max="5" width="11.3046875" customWidth="1"/>
+    <col min="6" max="6" width="14.765625" customWidth="1"/>
+    <col min="7" max="7" width="22.23046875" customWidth="1"/>
+    <col min="8" max="8" width="18.07421875" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="31.3046875" customWidth="1"/>
+    <col min="11" max="11" width="14.23046875" customWidth="1"/>
+    <col min="12" max="12" width="13.3046875" customWidth="1"/>
+    <col min="13" max="13" width="70.921875" customWidth="1"/>
+    <col min="14" max="30" width="10.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -874,9 +927,9 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -897,7 +950,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>19</v>
@@ -915,26 +968,26 @@
         <v>23</v>
       </c>
       <c r="N2" s="3"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+    </row>
+    <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>14</v>
@@ -973,26 +1026,26 @@
         <v>29</v>
       </c>
       <c r="N3" s="3"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+    </row>
+    <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
@@ -1013,7 +1066,7 @@
         <v>31</v>
       </c>
       <c r="H4" s="5">
-        <v>8.421691423225E12</v>
+        <v>8421691423225</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>19</v>
@@ -1031,31 +1084,31 @@
         <v>29</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" customHeight="1">
       <c r="A5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1064,14 +1117,14 @@
       <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="9">
-        <v>8.42169142322E11</v>
+      <c r="H5" s="5">
+        <v>842169142322</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>19</v>
@@ -1089,31 +1142,31 @@
         <v>29</v>
       </c>
       <c r="N5" s="3"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+    </row>
+    <row r="6" spans="1:30" ht="15.75" customHeight="1">
       <c r="A6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1122,14 +1175,14 @@
       <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="9">
-        <v>8.4216914232255E13</v>
+      <c r="H6" s="5">
+        <v>84216914232255</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>19</v>
@@ -1147,26 +1200,26 @@
         <v>29</v>
       </c>
       <c r="N6" s="3"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" customHeight="1">
       <c r="A7" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1181,26 +1234,26 @@
       <c r="L7" s="3"/>
       <c r="M7" s="5"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7"/>
-      <c r="AD7" s="7"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+    </row>
+    <row r="8" spans="1:30" ht="15.75" customHeight="1">
       <c r="A8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>14</v>
@@ -1221,7 +1274,7 @@
         <v>18</v>
       </c>
       <c r="H8" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>28</v>
@@ -1239,26 +1292,26 @@
         <v>38</v>
       </c>
       <c r="N8" s="3"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+    </row>
+    <row r="9" spans="1:30" ht="15.75" customHeight="1">
       <c r="A9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>14</v>
@@ -1279,7 +1332,7 @@
         <v>40</v>
       </c>
       <c r="H9" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>41</v>
@@ -1297,26 +1350,26 @@
         <v>42</v>
       </c>
       <c r="N9" s="3"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="7"/>
-    </row>
-    <row r="10" ht="16.5" customHeight="1">
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+    </row>
+    <row r="10" spans="1:30" ht="16.5" customHeight="1">
       <c r="A10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>14</v>
@@ -1333,14 +1386,14 @@
       <c r="F10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="3" t="s">
         <v>44</v>
       </c>
       <c r="H10" s="5">
-        <v>8.42169142322E12</v>
-      </c>
-      <c r="I10" s="9">
-        <v>3333.0</v>
+        <v>8421691423220</v>
+      </c>
+      <c r="I10" s="5">
+        <v>3333</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>20</v>
@@ -1355,26 +1408,26 @@
         <v>42</v>
       </c>
       <c r="N10" s="3"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="7"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="10">
-        <v>10.0</v>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+    </row>
+    <row r="11" spans="1:30" ht="15.75" customHeight="1">
+      <c r="A11" s="3">
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
@@ -1388,16 +1441,16 @@
       <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="5">
-        <v>8.42169142322E12</v>
-      </c>
-      <c r="I11" s="9" t="s">
+        <v>8421691423220</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="5" t="s">
@@ -1413,26 +1466,26 @@
         <v>42</v>
       </c>
       <c r="N11" s="3"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="7"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+    </row>
+    <row r="12" spans="1:30" ht="15.75" customHeight="1">
       <c r="A12" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1447,26 +1500,26 @@
       <c r="L12" s="3"/>
       <c r="M12" s="5"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="7"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="10">
-        <v>13.0</v>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+    </row>
+    <row r="13" spans="1:30" ht="15.75" customHeight="1">
+      <c r="A13" s="3">
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>14</v>
@@ -1474,20 +1527,20 @@
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="4" t="s">
         <v>47</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H13" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>28</v>
@@ -1505,26 +1558,26 @@
         <v>38</v>
       </c>
       <c r="N13" s="3"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="7"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+    </row>
+    <row r="14" spans="1:30" ht="15.75" customHeight="1">
       <c r="A14" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>14</v>
@@ -1532,26 +1585,26 @@
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H14" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="9">
-        <v>3333.0</v>
+      <c r="J14" s="5">
+        <v>3333</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>21</v>
@@ -1559,56 +1612,56 @@
       <c r="L14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="M14" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N14" s="3"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7"/>
-      <c r="AD14" s="7"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+    </row>
+    <row r="15" spans="1:30" ht="15.75" customHeight="1">
       <c r="A15" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="3" t="s">
         <v>53</v>
       </c>
       <c r="H15" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="7" t="s">
         <v>54</v>
       </c>
       <c r="K15" s="5" t="s">
@@ -1617,56 +1670,56 @@
       <c r="L15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="M15" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N15" s="3"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="7"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+    </row>
+    <row r="16" spans="1:30" ht="15.75" customHeight="1">
       <c r="A16" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="3" t="s">
         <v>56</v>
       </c>
       <c r="H16" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="7" t="s">
         <v>57</v>
       </c>
       <c r="K16" s="5" t="s">
@@ -1675,30 +1728,30 @@
       <c r="L16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="M16" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N16" s="3"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="7"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="7"/>
-      <c r="AD16" s="7"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+    </row>
+    <row r="17" spans="1:30" ht="15.75" customHeight="1">
       <c r="A17" s="3">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
@@ -1706,25 +1759,25 @@
       <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="3" t="s">
         <v>59</v>
       </c>
       <c r="H17" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K17" s="5" t="s">
@@ -1733,39 +1786,39 @@
       <c r="L17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="9" t="s">
+      <c r="M17" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N17" s="3"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
-      <c r="AA17" s="7"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+    </row>
+    <row r="18" spans="1:30" ht="15.75" customHeight="1">
       <c r="A18" s="3">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="8"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="10"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1773,47 +1826,47 @@
       <c r="L18" s="6"/>
       <c r="M18" s="5"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
-      <c r="AA18" s="7"/>
-      <c r="AB18" s="7"/>
-      <c r="AC18" s="7"/>
-      <c r="AD18" s="7"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+    </row>
+    <row r="19" spans="1:30" ht="15.75" customHeight="1">
       <c r="A19" s="3">
-        <v>18.0</v>
-      </c>
-      <c r="B19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H19" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>28</v>
@@ -1831,47 +1884,47 @@
         <v>38</v>
       </c>
       <c r="N19" s="3"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
-      <c r="Z19" s="7"/>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="7"/>
-      <c r="AC19" s="7"/>
-      <c r="AD19" s="7"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+    </row>
+    <row r="20" spans="1:30" ht="15.75" customHeight="1">
       <c r="A20" s="3">
-        <v>19.0</v>
-      </c>
-      <c r="B20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="3" t="s">
         <v>66</v>
       </c>
       <c r="H20" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>28</v>
@@ -1886,51 +1939,51 @@
       <c r="L20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M20" s="9" t="s">
+      <c r="M20" s="5" t="s">
         <v>67</v>
       </c>
       <c r="N20" s="3"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
-      <c r="Z20" s="7"/>
-      <c r="AA20" s="7"/>
-      <c r="AB20" s="7"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="7"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+    </row>
+    <row r="21" spans="1:30" ht="15.75" customHeight="1">
       <c r="A21" s="3">
-        <v>20.0</v>
-      </c>
-      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H21" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>28</v>
@@ -1938,57 +1991,57 @@
       <c r="J21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="5" t="s">
         <v>70</v>
       </c>
       <c r="L21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M21" s="9" t="s">
+      <c r="M21" s="5" t="s">
         <v>67</v>
       </c>
       <c r="N21" s="3"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="7"/>
-      <c r="Y21" s="7"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="7"/>
-      <c r="AB21" s="7"/>
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+    </row>
+    <row r="22" spans="1:30" ht="15.75" customHeight="1">
       <c r="A22" s="3">
-        <v>21.0</v>
-      </c>
-      <c r="B22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="3" t="s">
         <v>72</v>
       </c>
       <c r="H22" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>28</v>
@@ -1996,57 +2049,57 @@
       <c r="J22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K22" s="5" t="s">
         <v>73</v>
       </c>
       <c r="L22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M22" s="9" t="s">
+      <c r="M22" s="5" t="s">
         <v>67</v>
       </c>
       <c r="N22" s="3"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7"/>
-      <c r="AA22" s="7"/>
-      <c r="AB22" s="7"/>
-      <c r="AC22" s="7"/>
-      <c r="AD22" s="7"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+    </row>
+    <row r="23" spans="1:30" ht="15.75" customHeight="1">
       <c r="A23" s="3">
-        <v>22.0</v>
-      </c>
-      <c r="B23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H23" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>28</v>
@@ -2054,43 +2107,43 @@
       <c r="J23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="K23" s="5" t="s">
         <v>76</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="9" t="s">
+      <c r="M23" s="5" t="s">
         <v>67</v>
       </c>
       <c r="N23" s="3"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="7"/>
-      <c r="AB23" s="7"/>
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="7"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+    </row>
+    <row r="24" spans="1:30" ht="15.75" customHeight="1">
       <c r="A24" s="3">
-        <v>23.0</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -2098,47 +2151,47 @@
       <c r="L24" s="3"/>
       <c r="M24" s="5"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="7"/>
-      <c r="AB24" s="7"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="7"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+    </row>
+    <row r="25" spans="1:30" ht="15.75" customHeight="1">
       <c r="A25" s="3">
-        <v>24.0</v>
-      </c>
-      <c r="B25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H25" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>28</v>
@@ -2156,47 +2209,47 @@
         <v>38</v>
       </c>
       <c r="N25" s="3"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="7"/>
-      <c r="W25" s="7"/>
-      <c r="X25" s="7"/>
-      <c r="Y25" s="7"/>
-      <c r="Z25" s="7"/>
-      <c r="AA25" s="7"/>
-      <c r="AB25" s="7"/>
-      <c r="AC25" s="7"/>
-      <c r="AD25" s="7"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+    </row>
+    <row r="26" spans="1:30" ht="15.75" customHeight="1">
       <c r="A26" s="3">
-        <v>25.0</v>
-      </c>
-      <c r="B26" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="3" t="s">
         <v>79</v>
       </c>
       <c r="H26" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>28</v>
@@ -2207,54 +2260,54 @@
       <c r="K26" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L26" s="12" t="s">
+      <c r="L26" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="M26" s="9" t="s">
+      <c r="M26" s="5" t="s">
         <v>81</v>
       </c>
       <c r="N26" s="3"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
-      <c r="U26" s="7"/>
-      <c r="V26" s="7"/>
-      <c r="W26" s="7"/>
-      <c r="X26" s="7"/>
-      <c r="Y26" s="7"/>
-      <c r="Z26" s="7"/>
-      <c r="AA26" s="7"/>
-      <c r="AB26" s="7"/>
-      <c r="AC26" s="7"/>
-      <c r="AD26" s="7"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+    </row>
+    <row r="27" spans="1:30" ht="15.75" customHeight="1">
       <c r="A27" s="3">
-        <v>26.0</v>
-      </c>
-      <c r="B27" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="3" t="s">
         <v>83</v>
       </c>
       <c r="H27" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>28</v>
@@ -2265,54 +2318,54 @@
       <c r="K27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L27" s="12" t="s">
+      <c r="L27" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M27" s="9" t="s">
+      <c r="M27" s="5" t="s">
         <v>81</v>
       </c>
       <c r="N27" s="5"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-      <c r="AA27" s="13"/>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
-      <c r="AD27" s="13"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+    </row>
+    <row r="28" spans="1:30" ht="15.75" customHeight="1">
       <c r="A28" s="3">
-        <v>27.0</v>
-      </c>
-      <c r="B28" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="4" t="s">
         <v>85</v>
       </c>
       <c r="H28" s="5">
-        <v>8.42169142322E12</v>
+        <v>8421691423220</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>28</v>
@@ -2323,35 +2376,35 @@
       <c r="K28" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L28" s="12">
-        <v>28005.0</v>
-      </c>
-      <c r="M28" s="9" t="s">
+      <c r="L28" s="6">
+        <v>28005</v>
+      </c>
+      <c r="M28" s="5" t="s">
         <v>81</v>
       </c>
       <c r="N28" s="3"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-      <c r="V28" s="7"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="7"/>
-      <c r="Y28" s="7"/>
-      <c r="Z28" s="7"/>
-      <c r="AA28" s="7"/>
-      <c r="AB28" s="7"/>
-      <c r="AC28" s="7"/>
-      <c r="AD28" s="7"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+    </row>
+    <row r="29" spans="1:30" ht="15.75" customHeight="1">
       <c r="A29" s="3">
-        <v>28.0</v>
-      </c>
-      <c r="B29" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2364,26 +2417,26 @@
       <c r="L29" s="3"/>
       <c r="M29" s="5"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
-      <c r="W29" s="7"/>
-      <c r="X29" s="7"/>
-      <c r="Y29" s="7"/>
-      <c r="Z29" s="7"/>
-      <c r="AA29" s="7"/>
-      <c r="AB29" s="7"/>
-      <c r="AC29" s="7"/>
-      <c r="AD29" s="7"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+    </row>
+    <row r="30" spans="1:30" ht="15.75" customHeight="1">
       <c r="A30" s="3">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2398,26 +2451,26 @@
       <c r="L30" s="3"/>
       <c r="M30" s="5"/>
       <c r="N30" s="3"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="7"/>
-      <c r="W30" s="7"/>
-      <c r="X30" s="7"/>
-      <c r="Y30" s="7"/>
-      <c r="Z30" s="7"/>
-      <c r="AA30" s="7"/>
-      <c r="AB30" s="7"/>
-      <c r="AC30" s="7"/>
-      <c r="AD30" s="7"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+    </row>
+    <row r="31" spans="1:30" ht="15.75" customHeight="1">
       <c r="A31" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2432,26 +2485,26 @@
       <c r="L31" s="3"/>
       <c r="M31" s="5"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-      <c r="V31" s="7"/>
-      <c r="W31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="7"/>
-      <c r="AB31" s="7"/>
-      <c r="AC31" s="7"/>
-      <c r="AD31" s="7"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+    </row>
+    <row r="32" spans="1:30" ht="15.75" customHeight="1">
       <c r="A32" s="3">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2466,26 +2519,26 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
-      <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="7"/>
-      <c r="AA32" s="7"/>
-      <c r="AB32" s="7"/>
-      <c r="AC32" s="7"/>
-      <c r="AD32" s="7"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
+    </row>
+    <row r="33" spans="1:30" ht="15.75" customHeight="1">
       <c r="A33" s="3">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2500,24 +2553,24 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="7"/>
-      <c r="AC33" s="7"/>
-      <c r="AD33" s="7"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+    </row>
+    <row r="34" spans="1:30" ht="15.75" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>86</v>
@@ -2540,24 +2593,24 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="7"/>
-      <c r="V34" s="7"/>
-      <c r="W34" s="7"/>
-      <c r="X34" s="7"/>
-      <c r="Y34" s="7"/>
-      <c r="Z34" s="7"/>
-      <c r="AA34" s="7"/>
-      <c r="AB34" s="7"/>
-      <c r="AC34" s="7"/>
-      <c r="AD34" s="7"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="3"/>
+    </row>
+    <row r="35" spans="1:30" ht="15.75" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
         <v>86</v>
@@ -2580,24 +2633,24 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7"/>
-      <c r="T35" s="7"/>
-      <c r="U35" s="7"/>
-      <c r="V35" s="7"/>
-      <c r="W35" s="7"/>
-      <c r="X35" s="7"/>
-      <c r="Y35" s="7"/>
-      <c r="Z35" s="7"/>
-      <c r="AA35" s="7"/>
-      <c r="AB35" s="7"/>
-      <c r="AC35" s="7"/>
-      <c r="AD35" s="7"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="3"/>
+      <c r="AC35" s="3"/>
+      <c r="AD35" s="3"/>
+    </row>
+    <row r="36" spans="1:30" ht="15.75" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2612,24 +2665,24 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="7"/>
-      <c r="T36" s="7"/>
-      <c r="U36" s="7"/>
-      <c r="V36" s="7"/>
-      <c r="W36" s="7"/>
-      <c r="X36" s="7"/>
-      <c r="Y36" s="7"/>
-      <c r="Z36" s="7"/>
-      <c r="AA36" s="7"/>
-      <c r="AB36" s="7"/>
-      <c r="AC36" s="7"/>
-      <c r="AD36" s="7"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3"/>
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="3"/>
+    </row>
+    <row r="37" spans="1:30" ht="15.75" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2644,24 +2697,24 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
-      <c r="O37" s="7"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7"/>
-      <c r="R37" s="7"/>
-      <c r="S37" s="7"/>
-      <c r="T37" s="7"/>
-      <c r="U37" s="7"/>
-      <c r="V37" s="7"/>
-      <c r="W37" s="7"/>
-      <c r="X37" s="7"/>
-      <c r="Y37" s="7"/>
-      <c r="Z37" s="7"/>
-      <c r="AA37" s="7"/>
-      <c r="AB37" s="7"/>
-      <c r="AC37" s="7"/>
-      <c r="AD37" s="7"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="3"/>
+      <c r="AD37" s="3"/>
+    </row>
+    <row r="38" spans="1:30" ht="15.75" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -2676,24 +2729,24 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="7"/>
-      <c r="T38" s="7"/>
-      <c r="U38" s="7"/>
-      <c r="V38" s="7"/>
-      <c r="W38" s="7"/>
-      <c r="X38" s="7"/>
-      <c r="Y38" s="7"/>
-      <c r="Z38" s="7"/>
-      <c r="AA38" s="7"/>
-      <c r="AB38" s="7"/>
-      <c r="AC38" s="7"/>
-      <c r="AD38" s="7"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3"/>
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="3"/>
+    </row>
+    <row r="39" spans="1:30" ht="15.75" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2708,24 +2761,24 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="7"/>
-      <c r="V39" s="7"/>
-      <c r="W39" s="7"/>
-      <c r="X39" s="7"/>
-      <c r="Y39" s="7"/>
-      <c r="Z39" s="7"/>
-      <c r="AA39" s="7"/>
-      <c r="AB39" s="7"/>
-      <c r="AC39" s="7"/>
-      <c r="AD39" s="7"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="3"/>
+    </row>
+    <row r="40" spans="1:30" ht="15.75" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2740,24 +2793,24 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="7"/>
-      <c r="T40" s="7"/>
-      <c r="U40" s="7"/>
-      <c r="V40" s="7"/>
-      <c r="W40" s="7"/>
-      <c r="X40" s="7"/>
-      <c r="Y40" s="7"/>
-      <c r="Z40" s="7"/>
-      <c r="AA40" s="7"/>
-      <c r="AB40" s="7"/>
-      <c r="AC40" s="7"/>
-      <c r="AD40" s="7"/>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3"/>
+      <c r="AC40" s="3"/>
+      <c r="AD40" s="3"/>
+    </row>
+    <row r="41" spans="1:30" ht="15.75" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2772,24 +2825,24 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
-      <c r="T41" s="7"/>
-      <c r="U41" s="7"/>
-      <c r="V41" s="7"/>
-      <c r="W41" s="7"/>
-      <c r="X41" s="7"/>
-      <c r="Y41" s="7"/>
-      <c r="Z41" s="7"/>
-      <c r="AA41" s="7"/>
-      <c r="AB41" s="7"/>
-      <c r="AC41" s="7"/>
-      <c r="AD41" s="7"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Y41" s="3"/>
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="3"/>
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="3"/>
+    </row>
+    <row r="42" spans="1:30" ht="15.75" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2804,24 +2857,24 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="7"/>
-      <c r="U42" s="7"/>
-      <c r="V42" s="7"/>
-      <c r="W42" s="7"/>
-      <c r="X42" s="7"/>
-      <c r="Y42" s="7"/>
-      <c r="Z42" s="7"/>
-      <c r="AA42" s="7"/>
-      <c r="AB42" s="7"/>
-      <c r="AC42" s="7"/>
-      <c r="AD42" s="7"/>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="3"/>
+    </row>
+    <row r="43" spans="1:30" ht="15.75" customHeight="1">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -2835,24 +2888,24 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="7"/>
-      <c r="T43" s="7"/>
-      <c r="U43" s="7"/>
-      <c r="V43" s="7"/>
-      <c r="W43" s="7"/>
-      <c r="X43" s="7"/>
-      <c r="Y43" s="7"/>
-      <c r="Z43" s="7"/>
-      <c r="AA43" s="7"/>
-      <c r="AB43" s="7"/>
-      <c r="AC43" s="7"/>
-      <c r="AD43" s="7"/>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Y43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="3"/>
+      <c r="AC43" s="3"/>
+      <c r="AD43" s="3"/>
+    </row>
+    <row r="44" spans="1:30" ht="15.75" customHeight="1">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -2866,27 +2919,27 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
-      <c r="S44" s="7"/>
-      <c r="T44" s="7"/>
-      <c r="U44" s="7"/>
-      <c r="V44" s="7"/>
-      <c r="W44" s="7"/>
-      <c r="X44" s="7"/>
-      <c r="Y44" s="7"/>
-      <c r="Z44" s="7"/>
-      <c r="AA44" s="7"/>
-      <c r="AB44" s="7"/>
-      <c r="AC44" s="7"/>
-      <c r="AD44" s="7"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3"/>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3"/>
+      <c r="AC44" s="3"/>
+      <c r="AD44" s="3"/>
+    </row>
+    <row r="45" spans="1:30" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:30" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:30" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:30" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -3841,93 +3894,89 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="10.1" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="10.07421875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="10.6"/>
-    <col customWidth="1" min="3" max="3" width="26.6"/>
-    <col customWidth="1" min="4" max="4" width="44.1"/>
-    <col customWidth="1" min="5" max="5" width="22.3"/>
-    <col customWidth="1" min="6" max="6" width="62.3"/>
-    <col customWidth="1" min="7" max="7" width="9.3"/>
-    <col customWidth="1" min="8" max="8" width="36.7"/>
-    <col customWidth="1" min="9" max="10" width="33.7"/>
-    <col customWidth="1" min="11" max="28" width="10.6"/>
+    <col min="1" max="2" width="10.61328125" customWidth="1"/>
+    <col min="3" max="3" width="26.61328125" customWidth="1"/>
+    <col min="4" max="4" width="44.07421875" customWidth="1"/>
+    <col min="5" max="5" width="22.3046875" customWidth="1"/>
+    <col min="6" max="6" width="62.3046875" customWidth="1"/>
+    <col min="7" max="7" width="9.3046875" customWidth="1"/>
+    <col min="8" max="8" width="36.69140625" customWidth="1"/>
+    <col min="9" max="10" width="33.69140625" customWidth="1"/>
+    <col min="11" max="28" width="10.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="33.0" customHeight="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:28" ht="33" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>97</v>
@@ -3952,9 +4001,9 @@
       </c>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3966,9 +4015,9 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
       <c r="A4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3980,9 +4029,9 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:28" ht="15.75" customHeight="1">
       <c r="A5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3994,9 +4043,9 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:28" ht="15.75" customHeight="1">
       <c r="A6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -4008,7 +4057,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -4020,7 +4069,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -4032,7 +4081,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:28" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4044,7 +4093,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:28" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4056,7 +4105,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:28" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -4068,7 +4117,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:28" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -4080,7 +4129,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:28" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4092,7 +4141,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4104,7 +4153,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:28" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -4116,7 +4165,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -4128,7 +4177,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -4140,7 +4189,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4152,7 +4201,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4164,7 +4213,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -4176,7 +4225,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4188,7 +4237,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4200,7 +4249,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4212,7 +4261,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4224,7 +4273,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4236,7 +4285,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4248,7 +4297,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4260,7 +4309,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4272,7 +4321,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4284,7 +4333,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4296,7 +4345,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4308,7 +4357,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4320,7 +4369,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4332,7 +4381,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4344,7 +4393,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4356,7 +4405,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4368,7 +4417,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4380,7 +4429,7 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4392,7 +4441,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -4404,7 +4453,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -4416,7 +4465,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -4428,7 +4477,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -4440,7 +4489,7 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -4452,11 +4501,11 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -5410,36 +5459,32 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="10.1" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="10.07421875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.6"/>
-    <col customWidth="1" min="2" max="2" width="15.6"/>
-    <col customWidth="1" min="3" max="3" width="22.3"/>
-    <col customWidth="1" min="4" max="4" width="62.3"/>
-    <col customWidth="1" min="5" max="5" width="9.3"/>
-    <col customWidth="1" min="6" max="7" width="33.7"/>
-    <col customWidth="1" min="8" max="25" width="10.6"/>
+    <col min="1" max="1" width="10.61328125" customWidth="1"/>
+    <col min="2" max="2" width="15.61328125" customWidth="1"/>
+    <col min="3" max="3" width="22.3046875" customWidth="1"/>
+    <col min="4" max="4" width="62.3046875" customWidth="1"/>
+    <col min="5" max="5" width="9.3046875" customWidth="1"/>
+    <col min="6" max="7" width="33.69140625" customWidth="1"/>
+    <col min="8" max="25" width="10.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5462,9 +5507,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>105</v>
@@ -5477,9 +5522,9 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5488,9 +5533,9 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -5499,9 +5544,9 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -5510,9 +5555,9 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -5521,7 +5566,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -5530,7 +5575,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -5539,7 +5584,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -5548,7 +5593,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5557,7 +5602,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -5566,7 +5611,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5575,7 +5620,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -5584,7 +5629,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -5593,7 +5638,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -5602,7 +5647,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -5611,7 +5656,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -5620,7 +5665,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -5629,7 +5674,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -5638,7 +5683,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -5647,7 +5692,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -5656,7 +5701,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5665,7 +5710,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5674,7 +5719,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5683,7 +5728,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5692,7 +5737,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5701,7 +5746,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5710,7 +5755,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5719,7 +5764,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5728,7 +5773,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5737,7 +5782,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5746,7 +5791,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5755,7 +5800,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5764,7 +5809,7 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:7" ht="15.75" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5773,7 +5818,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:7" ht="15.75" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5782,7 +5827,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:7" ht="15.75" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5791,7 +5836,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:7" ht="15.75" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5800,7 +5845,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:7" ht="15.75" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5809,7 +5854,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:7" ht="15.75" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -5818,7 +5863,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:7" ht="15.75" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -5827,7 +5872,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -5836,7 +5881,7 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:7" ht="15.75" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5845,7 +5890,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:7" ht="15.75" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -5854,11 +5899,11 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -6812,12 +6857,10 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>